<commit_message>
nuevo cambio en IPC calculado
</commit_message>
<xml_diff>
--- a/IPC_Evolucion_conApertura.xlsx
+++ b/IPC_Evolucion_conApertura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db46ee0f0451afdd/Academico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{7E258CFC-FADC-49A7-B615-4528C9943B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="14_{7E258CFC-FADC-49A7-B615-4528C9943B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7BD2D54-52EC-4A04-A714-66165BD7298F}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68960CE0-F17F-4628-A9C8-3A1003AD9D3E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>01</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Mes_final</t>
+  </si>
+  <si>
+    <t>Indice_Final</t>
+  </si>
+  <si>
+    <t>Var Anual</t>
   </si>
 </sst>
 </file>
@@ -171,10 +177,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,15 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8279CA40-A1A2-46A2-9732-C9ADF944E8AB}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
@@ -494,16 +496,25 @@
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -531,8 +542,17 @@
       <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43100</v>
       </c>
@@ -550,8 +570,24 @@
         <f>E4/(1.11)</f>
         <v>174.61261261261259</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <f>A3</f>
+        <v>43100</v>
+      </c>
+      <c r="G3" s="2">
+        <f>C3</f>
+        <v>172.86</v>
+      </c>
+      <c r="H3" s="2">
+        <f>D3</f>
+        <v>178.81625772616593</v>
+      </c>
+      <c r="I3" s="2">
+        <f>E3</f>
+        <v>174.61261261261259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43465</v>
       </c>
@@ -571,20 +607,32 @@
         <f>A4</f>
         <v>43465</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:I12" si="0">C4</f>
+        <v>186.62</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>190.94</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>193.82</v>
+      </c>
+      <c r="J4" s="3">
         <f>C4/C3-1</f>
         <v>7.9601990049751103E-2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="K4" s="3">
         <f>D4/D3-1</f>
         <v>6.7800000000000082E-2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="L4" s="3">
         <f>E4/E3-1</f>
         <v>0.1100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43646</v>
       </c>
@@ -604,20 +652,32 @@
         <f>A5</f>
         <v>43646</v>
       </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:I11" si="0">C5/C3-1</f>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>196.44</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>200.49</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>205.78</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" ref="J5:L11" si="1">C5/C3-1</f>
         <v>0.13641096841374512</v>
       </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
         <v>0.12120677699801008</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" si="0"/>
+      <c r="L5" s="3">
+        <f t="shared" si="1"/>
         <v>0.17849447941388941</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43830</v>
       </c>
@@ -637,20 +697,32 @@
         <f>A6</f>
         <v>43830</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>203.02</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>218.06</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>208.26</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
         <v>8.7879112635301793E-2</v>
       </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
         <v>0.14203414685241444</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="0"/>
+      <c r="L6" s="3">
+        <f t="shared" si="1"/>
         <v>7.450211536477136E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44012</v>
       </c>
@@ -670,20 +742,32 @@
         <f>A7</f>
         <v>44012</v>
       </c>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>216.8</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>233.84</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>225.9</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
         <v>0.10364487884341278</v>
       </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
         <v>0.16634246097062189</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="0"/>
+      <c r="L7" s="3">
+        <f t="shared" si="1"/>
         <v>9.7774322091554122E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44196</v>
       </c>
@@ -702,20 +786,32 @@
       <c r="F8" s="1">
         <v>44196</v>
       </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>222.13</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>238.73</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>229.99</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
         <v>9.4128657275145189E-2</v>
       </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
         <v>9.4790424653764971E-2</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
         <v>0.10434072793623361</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44377</v>
       </c>
@@ -735,20 +831,32 @@
         <f>A9</f>
         <v>44377</v>
       </c>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>232.69</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>246.81</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>248.14</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
         <v>7.3293357933579273E-2</v>
       </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
         <v>5.5465275401984204E-2</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
         <v>9.845064187693664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44561</v>
       </c>
@@ -767,20 +875,32 @@
       <c r="F10" s="1">
         <v>44561</v>
       </c>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>239.80600000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>254.25</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>251.44</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
         <v>7.9575023634808506E-2</v>
       </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
         <v>6.5010681523059555E-2</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
+      <c r="L10" s="3">
+        <f t="shared" si="1"/>
         <v>9.3264924561937468E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44742</v>
       </c>
@@ -800,20 +920,32 @@
         <f>A11</f>
         <v>44742</v>
       </c>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>254.3</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>273.58999999999997</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>264.77999999999997</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
         <v>9.2870342515793514E-2</v>
       </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
         <v>0.10850451764515201</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
+      <c r="L11" s="3">
+        <f t="shared" si="1"/>
         <v>6.7058918352542962E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44865</v>
       </c>
@@ -829,8 +961,24 @@
       <c r="E12" s="2">
         <v>267.60000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <f>A12</f>
+        <v>44865</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>261.10489999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>284.2</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>267.60000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44865</v>
       </c>
@@ -846,8 +994,11 @@
       <c r="E13" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44926</v>
       </c>
@@ -855,7 +1006,7 @@
         <v>44865</v>
       </c>
       <c r="C14" s="2">
-        <v>99.465050000000005</v>
+        <v>99.465010000000007</v>
       </c>
       <c r="D14" s="2">
         <v>100</v>
@@ -866,18 +1017,78 @@
       <c r="F14" s="1">
         <v>44926</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
+        <f>C14/C$13*C$12</f>
+        <v>259.70801489549001</v>
+      </c>
+      <c r="H14" s="2">
+        <f>D14/D$13*D$12</f>
+        <v>284.2</v>
+      </c>
+      <c r="I14" s="2">
+        <f>E14/E$13*E$12</f>
+        <v>268.45632000000001</v>
+      </c>
+      <c r="J14" s="3">
         <f>(1+(C12/C10-1))*(1+(C14/C13-1))-1</f>
-        <v>8.2992582910561108E-2</v>
-      </c>
-      <c r="H14" s="3">
+        <v>8.2992147383676773E-2</v>
+      </c>
+      <c r="K14" s="3">
         <f>(1+(D12/D10-1))*(1+(D14/D13-1))-1</f>
         <v>0.11779744346116017</v>
       </c>
-      <c r="I14" s="3">
+      <c r="L14" s="3">
         <f>(1+(E12/E10-1))*(1+(E14/E13-1))-1</f>
         <v>6.7675469296850199E-2</v>
       </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44865</v>
+      </c>
+      <c r="C15" s="2">
+        <v>103.22</v>
+      </c>
+      <c r="D15" s="2">
+        <v>106.10509999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <v>104.84</v>
+      </c>
+      <c r="F15" s="1">
+        <f>A15</f>
+        <v>45107</v>
+      </c>
+      <c r="G15" s="2">
+        <f>C15/C$13*C$12</f>
+        <v>269.51247777999998</v>
+      </c>
+      <c r="H15" s="2">
+        <f>D15/D$13*D$12</f>
+        <v>301.55069419999995</v>
+      </c>
+      <c r="I15" s="2">
+        <f>E15/E$13*E$12</f>
+        <v>280.55184000000003</v>
+      </c>
+      <c r="J15" s="3">
+        <f>G15/G11-1</f>
+        <v>5.9820990090444282E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <f>H15/H11-1</f>
+        <v>0.10219925508973282</v>
+      </c>
+      <c r="L15" s="3">
+        <f>I15/I11-1</f>
+        <v>5.9565828234761087E-2</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>

</xml_diff>